<commit_message>
solved problem splitting line coordinates
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -424,39 +424,24 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>-57.75229665737701</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>-30.86397242051519</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>0</t>
+          <t>Points</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>-57.75285839699505</t>
+          <t>-57.75229665737701</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>-30.85975540560617</t>
+          <t>-30.86397242051519</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -468,17 +453,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>-57.75526384350523</t>
+          <t>-57.75285839699505</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>-30.84392242816692</t>
+          <t>-30.85975540560617</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -490,20 +475,42 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>-57.75526384350523</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>-30.84392242816692</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
           <t>3</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="B5" t="inlineStr">
         <is>
           <t>-57.75354348580155</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="C5" t="inlineStr">
         <is>
           <t>-30.85513424867982</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="D5" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -512,14 +519,22 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Lines</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Shapes</t>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>-57.75428294205687</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>-30.84993317123787</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>

</xml_diff>